<commit_message>
Add Ausgrid ZS Mascot Data
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z5404477\Documents\PyNNLF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DAE1F5-5FB1-48C2-843B-5139FEE35D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FADC05-83FC-4259-B86C-8BF204216786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -195,16 +195,48 @@
   </si>
   <si>
     <t>ds0_test</t>
+  </si>
+  <si>
+    <t>ds14_ausgrid_zs_mascot</t>
+  </si>
+  <si>
+    <t>Ausgrid Zone Substation Data Mascot 33_11kV from FY2006 to FY2024</t>
+  </si>
+  <si>
+    <t>19 years</t>
+  </si>
+  <si>
+    <t>15 minute</t>
+  </si>
+  <si>
+    <t>https://www.ausgrid.com.au/Industry/Our-Research/Data-to-share/Distribution-zone-substation-data</t>
+  </si>
+  <si>
+    <t>ds15_ausgrid_zs_mascot_30min_with_weather</t>
+  </si>
+  <si>
+    <t>ds14 but converted to 30-minutely, added with BOM weather data, and filtered to 3 years</t>
+  </si>
+  <si>
+    <t>Use Sydney Airport weather data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -227,14 +259,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -258,8 +293,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C147F41-EE5B-49BB-8BD7-D0A566A629F0}" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{0C147F41-EE5B-49BB-8BD7-D0A566A629F0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C147F41-EE5B-49BB-8BD7-D0A566A629F0}" name="Table1" displayName="Table1" ref="A1:I17" totalsRowShown="0">
+  <autoFilter ref="A1:I17" xr:uid="{0C147F41-EE5B-49BB-8BD7-D0A566A629F0}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0AC41CFD-BE4C-4469-A375-569568B3D7FF}" name="name"/>
     <tableColumn id="2" xr3:uid="{F58FFEFF-0AFF-41A1-B30B-DE149B39B65A}" name="description"/>
@@ -538,17 +573,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="38.3515625" customWidth="1"/>
-    <col min="2" max="2" width="65.8203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.8203125" customWidth="1"/>
+    <col min="2" max="2" width="107.76171875" customWidth="1"/>
+    <col min="3" max="3" width="67.52734375" customWidth="1"/>
     <col min="5" max="5" width="10.29296875" customWidth="1"/>
     <col min="6" max="6" width="9.703125" customWidth="1"/>
     <col min="9" max="9" width="100.9375" bestFit="1" customWidth="1"/>
@@ -983,10 +1018,71 @@
         <v>48</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1">
+        <v>38473</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45412</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44013</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45107</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I16" r:id="rId1" xr:uid="{DEE855BE-FD64-4A90-8404-918F524DE7CB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>